<commit_message>
Add all tables excel for DB to import
</commit_message>
<xml_diff>
--- a/Data/paper/paper.xlsx
+++ b/Data/paper/paper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1476" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="1932" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -682,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,11 +756,11 @@
       </c>
       <c r="G2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <f ca="1">RANDBETWEEN(1, 5)+RANDBETWEEN(1,9)/10</f>
-        <v>5.3</v>
+        <v>4.3</v>
       </c>
       <c r="I2" t="s">
         <v>44</v>
@@ -773,7 +773,7 @@
       </c>
       <c r="L2" s="2">
         <f ca="1">DATE(RANDBETWEEN(2000,2020), RANDBETWEEN(1,12), DAY(RANDBETWEEN(1,28)))</f>
-        <v>39118</v>
+        <v>43601</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="72" x14ac:dyDescent="0.3">
@@ -794,15 +794,15 @@
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G51" ca="1" si="1">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H51" ca="1" si="2">RANDBETWEEN(1, 5)+RANDBETWEEN(1,9)/10</f>
-        <v>4.4000000000000004</v>
+        <v>1.5</v>
       </c>
       <c r="I3" t="s">
         <v>45</v>
@@ -815,7 +815,7 @@
       </c>
       <c r="L3" s="2">
         <f t="shared" ref="L3:L51" ca="1" si="3">DATE(RANDBETWEEN(2000,2020), RANDBETWEEN(1,12), DAY(RANDBETWEEN(1,28)))</f>
-        <v>37380</v>
+        <v>39570</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="72" x14ac:dyDescent="0.3">
@@ -840,11 +840,11 @@
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="2"/>
-        <v>4.8</v>
+        <v>3.7</v>
       </c>
       <c r="I4" t="s">
         <v>46</v>
@@ -857,7 +857,7 @@
       </c>
       <c r="L4" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>42145</v>
+        <v>37492</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -882,7 +882,7 @@
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="2"/>
@@ -899,7 +899,7 @@
       </c>
       <c r="L5" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>38345</v>
+        <v>42085</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -920,15 +920,15 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="2"/>
-        <v>5.8</v>
+        <v>3.6</v>
       </c>
       <c r="I6" t="s">
         <v>45</v>
@@ -941,7 +941,7 @@
       </c>
       <c r="L6" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>37124</v>
+        <v>42629</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
@@ -962,15 +962,15 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="2"/>
-        <v>2.9</v>
+        <v>2.4</v>
       </c>
       <c r="I7" t="s">
         <v>45</v>
@@ -983,7 +983,7 @@
       </c>
       <c r="L7" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>41106</v>
+        <v>43641</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -1004,15 +1004,15 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ca="1" si="1"/>
         <v>2</v>
       </c>
-      <c r="G8">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
       <c r="H8">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>3.1</v>
       </c>
       <c r="I8" t="s">
         <v>46</v>
@@ -1025,7 +1025,7 @@
       </c>
       <c r="L8" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>44044</v>
+        <v>39439</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
@@ -1046,15 +1046,15 @@
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="2"/>
-        <v>2.8</v>
+        <v>4.2</v>
       </c>
       <c r="I9" t="s">
         <v>45</v>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="L9" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>42596</v>
+        <v>36717</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="72" x14ac:dyDescent="0.3">
@@ -1088,15 +1088,15 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="2"/>
-        <v>5.2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I10" t="s">
         <v>45</v>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="L10" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>39407</v>
+        <v>41518</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -1130,7 +1130,7 @@
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="1"/>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="2"/>
-        <v>3.6</v>
+        <v>1.9</v>
       </c>
       <c r="I11" t="s">
         <v>44</v>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="L11" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>36977</v>
+        <v>42934</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -1172,15 +1172,15 @@
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="2"/>
-        <v>2.9</v>
+        <v>3.7</v>
       </c>
       <c r="I12" t="s">
         <v>45</v>
@@ -1193,7 +1193,7 @@
       </c>
       <c r="L12" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>43459</v>
+        <v>41025</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="72" x14ac:dyDescent="0.3">
@@ -1214,15 +1214,15 @@
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="2"/>
-        <v>1.7</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I13" t="s">
         <v>46</v>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="L13" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>39670</v>
+        <v>41606</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -1256,15 +1256,15 @@
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="2"/>
-        <v>1.9</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I14" t="s">
         <v>45</v>
@@ -1277,7 +1277,7 @@
       </c>
       <c r="L14" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>39969</v>
+        <v>41946</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
@@ -1298,15 +1298,15 @@
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="2"/>
-        <v>3.2</v>
+        <v>5.6</v>
       </c>
       <c r="I15" t="s">
         <v>45</v>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="L15" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>41197</v>
+        <v>43549</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -1344,11 +1344,11 @@
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="2"/>
-        <v>3.6</v>
+        <v>2.8</v>
       </c>
       <c r="I16" t="s">
         <v>47</v>
@@ -1361,7 +1361,7 @@
       </c>
       <c r="L16" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>36643</v>
+        <v>37962</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -1382,7 +1382,7 @@
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="2"/>
-        <v>2.4</v>
+        <v>4.7</v>
       </c>
       <c r="I17" t="s">
         <v>45</v>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="L17" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>40087</v>
+        <v>37782</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -1428,11 +1428,11 @@
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="2"/>
-        <v>4.3</v>
+        <v>1.8</v>
       </c>
       <c r="I18" t="s">
         <v>45</v>
@@ -1445,7 +1445,7 @@
       </c>
       <c r="L18" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>40963</v>
+        <v>38900</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -1466,15 +1466,15 @@
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="2"/>
-        <v>2.5</v>
+        <v>1.4</v>
       </c>
       <c r="I19" t="s">
         <v>48</v>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="L19" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>41934</v>
+        <v>44034</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -1512,11 +1512,11 @@
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="2"/>
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
       <c r="I20" t="s">
         <v>45</v>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="L20" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>41595</v>
+        <v>40170</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -1550,15 +1550,15 @@
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ca="1" si="1"/>
         <v>4</v>
       </c>
-      <c r="G21">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
       <c r="H21">
         <f t="shared" ca="1" si="2"/>
-        <v>3.6</v>
+        <v>1.6</v>
       </c>
       <c r="I21" t="s">
         <v>47</v>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="L21" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>41370</v>
+        <v>40101</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -1592,15 +1592,15 @@
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="2"/>
-        <v>3.5</v>
+        <v>1.2</v>
       </c>
       <c r="I22" t="s">
         <v>45</v>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="L22" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>39226</v>
+        <v>43523</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -1634,15 +1634,15 @@
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="2"/>
-        <v>2.1</v>
+        <v>2.4</v>
       </c>
       <c r="I23" t="s">
         <v>45</v>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="L23" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>39365</v>
+        <v>43999</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -1676,15 +1676,15 @@
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="2"/>
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="I24" t="s">
         <v>47</v>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="L24" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>38498</v>
+        <v>38887</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -1718,15 +1718,15 @@
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="2"/>
-        <v>3.6</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I25" t="s">
         <v>45</v>
@@ -1739,7 +1739,7 @@
       </c>
       <c r="L25" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>43659</v>
+        <v>39710</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="72" x14ac:dyDescent="0.3">
@@ -1760,7 +1760,7 @@
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="1"/>
@@ -1768,7 +1768,7 @@
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="2"/>
-        <v>3.7</v>
+        <v>2.9</v>
       </c>
       <c r="I26" t="s">
         <v>46</v>
@@ -1781,7 +1781,7 @@
       </c>
       <c r="L26" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>43392</v>
+        <v>36650</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
@@ -1806,11 +1806,11 @@
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="2"/>
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="I27" t="s">
         <v>45</v>
@@ -1823,7 +1823,7 @@
       </c>
       <c r="L27" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>41641</v>
+        <v>42330</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="72" x14ac:dyDescent="0.3">
@@ -1848,11 +1848,11 @@
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="2"/>
-        <v>1.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I28" t="s">
         <v>47</v>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="L28" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>42408</v>
+        <v>40409</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -1886,15 +1886,15 @@
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="2"/>
-        <v>5.6</v>
+        <v>5.8</v>
       </c>
       <c r="I29" t="s">
         <v>45</v>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="L29" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>44097</v>
+        <v>41778</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
@@ -1928,15 +1928,15 @@
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="2"/>
-        <v>3.7</v>
+        <v>1.5</v>
       </c>
       <c r="I30" t="s">
         <v>45</v>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="L30" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>37904</v>
+        <v>40538</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="72" x14ac:dyDescent="0.3">
@@ -1970,15 +1970,15 @@
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="2"/>
-        <v>3.7</v>
+        <v>4.5</v>
       </c>
       <c r="I31" t="s">
         <v>48</v>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="L31" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>43426</v>
+        <v>38670</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -2012,15 +2012,15 @@
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0999999999999996</v>
+        <v>3.8</v>
       </c>
       <c r="I32" t="s">
         <v>45</v>
@@ -2033,7 +2033,7 @@
       </c>
       <c r="L32" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>40201</v>
+        <v>42628</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -2054,15 +2054,15 @@
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="2"/>
-        <v>2.6</v>
+        <v>1.2</v>
       </c>
       <c r="I33" t="s">
         <v>45</v>
@@ -2075,7 +2075,7 @@
       </c>
       <c r="L33" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>41862</v>
+        <v>39047</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
@@ -2096,15 +2096,15 @@
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="2"/>
-        <v>2.8</v>
+        <v>3.7</v>
       </c>
       <c r="I34" t="s">
         <v>45</v>
@@ -2117,7 +2117,7 @@
       </c>
       <c r="L34" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>36781</v>
+        <v>37943</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -2138,15 +2138,15 @@
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H35">
         <f ca="1">RANDBETWEEN(1, 5)+RANDBETWEEN(1,9)/10</f>
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="I35" t="s">
         <v>48</v>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="L35" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>40638</v>
+        <v>37606</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -2180,15 +2180,15 @@
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="2"/>
-        <v>2.6</v>
+        <v>1.5</v>
       </c>
       <c r="I36" t="s">
         <v>45</v>
@@ -2201,7 +2201,7 @@
       </c>
       <c r="L36" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>42736</v>
+        <v>41165</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
@@ -2222,15 +2222,15 @@
       </c>
       <c r="F37">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G37">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="I37" t="s">
         <v>45</v>
@@ -2243,7 +2243,7 @@
       </c>
       <c r="L37" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>40622</v>
+        <v>43053</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
@@ -2264,15 +2264,15 @@
       </c>
       <c r="F38">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G38">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="2"/>
-        <v>1.2</v>
+        <v>4.7</v>
       </c>
       <c r="I38" t="s">
         <v>46</v>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="L38" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>42071</v>
+        <v>41062</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="72" x14ac:dyDescent="0.3">
@@ -2310,11 +2310,11 @@
       </c>
       <c r="G39">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="2"/>
-        <v>1.2</v>
+        <v>4.5</v>
       </c>
       <c r="I39" t="s">
         <v>47</v>
@@ -2327,7 +2327,7 @@
       </c>
       <c r="L39" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>38825</v>
+        <v>40138</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
@@ -2348,7 +2348,7 @@
       </c>
       <c r="F40">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G40">
         <f t="shared" ca="1" si="1"/>
@@ -2356,7 +2356,7 @@
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="2"/>
-        <v>4.2</v>
+        <v>2.6</v>
       </c>
       <c r="I40" t="s">
         <v>45</v>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="L40" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>41955</v>
+        <v>42401</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -2390,15 +2390,15 @@
       </c>
       <c r="F41">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G41">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="2"/>
-        <v>1.8</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I41" t="s">
         <v>45</v>
@@ -2411,7 +2411,7 @@
       </c>
       <c r="L41" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>43888</v>
+        <v>36989</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
@@ -2432,15 +2432,15 @@
       </c>
       <c r="F42">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G42">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="2"/>
-        <v>4.5</v>
+        <v>2.4</v>
       </c>
       <c r="I42" t="s">
         <v>45</v>
@@ -2453,7 +2453,7 @@
       </c>
       <c r="L42" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>40099</v>
+        <v>41508</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
@@ -2474,15 +2474,15 @@
       </c>
       <c r="F43">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G43">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="2"/>
-        <v>5.5</v>
+        <v>1.8</v>
       </c>
       <c r="I43" t="s">
         <v>47</v>
@@ -2495,7 +2495,7 @@
       </c>
       <c r="L43" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>37252</v>
+        <v>39661</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="72" x14ac:dyDescent="0.3">
@@ -2516,15 +2516,15 @@
       </c>
       <c r="F44">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G44">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="2"/>
-        <v>5.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I44" t="s">
         <v>46</v>
@@ -2537,7 +2537,7 @@
       </c>
       <c r="L44" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>42091</v>
+        <v>41448</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
@@ -2558,15 +2558,15 @@
       </c>
       <c r="F45">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G45">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="2"/>
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="I45" t="s">
         <v>45</v>
@@ -2579,7 +2579,7 @@
       </c>
       <c r="L45" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>39775</v>
+        <v>42989</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
@@ -2600,15 +2600,15 @@
       </c>
       <c r="F46">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G46">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="2"/>
-        <v>4.3</v>
+        <v>4.8</v>
       </c>
       <c r="I46" t="s">
         <v>45</v>
@@ -2621,7 +2621,7 @@
       </c>
       <c r="L46" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>37142</v>
+        <v>36621</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2642,11 +2642,11 @@
       </c>
       <c r="F47">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G47">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="2"/>
@@ -2663,7 +2663,7 @@
       </c>
       <c r="L47" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>36752</v>
+        <v>42892</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
@@ -2684,7 +2684,7 @@
       </c>
       <c r="F48">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G48">
         <f t="shared" ca="1" si="1"/>
@@ -2692,7 +2692,7 @@
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="2"/>
-        <v>4.7</v>
+        <v>2.4</v>
       </c>
       <c r="I48" t="s">
         <v>45</v>
@@ -2705,7 +2705,7 @@
       </c>
       <c r="L48" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>41366</v>
+        <v>36877</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="F49">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G49">
         <f t="shared" ca="1" si="1"/>
@@ -2734,7 +2734,7 @@
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="2"/>
-        <v>5.3</v>
+        <v>2.9</v>
       </c>
       <c r="I49" t="s">
         <v>45</v>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="L49" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>36563</v>
+        <v>42191</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
@@ -2768,15 +2768,15 @@
       </c>
       <c r="F50">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G50">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="2"/>
-        <v>2.9</v>
+        <v>1.6</v>
       </c>
       <c r="I50" t="s">
         <v>47</v>
@@ -2789,7 +2789,7 @@
       </c>
       <c r="L50" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>38371</v>
+        <v>43704</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -2810,15 +2810,15 @@
       </c>
       <c r="F51">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G51">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="2"/>
-        <v>2.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I51" t="s">
         <v>45</v>
@@ -2831,7 +2831,7 @@
       </c>
       <c r="L51" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>38829</v>
+        <v>37401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>